<commit_message>
Case Study 1 done
</commit_message>
<xml_diff>
--- a/PatientMonitors.xlsx
+++ b/PatientMonitors.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="90">
   <si>
     <t>Vitals and ECG</t>
   </si>
@@ -182,15 +182,6 @@
     <t>null</t>
   </si>
   <si>
-    <t>portablity_true</t>
-  </si>
-  <si>
-    <t>feature_true</t>
-  </si>
-  <si>
-    <t>size_true</t>
-  </si>
-  <si>
     <t>true</t>
   </si>
   <si>
@@ -291,6 +282,18 @@
   </si>
   <si>
     <t>Suresight VM1</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>portablity_1</t>
+  </si>
+  <si>
+    <t>feature_1</t>
+  </si>
+  <si>
+    <t>size_1</t>
   </si>
 </sst>
 </file>
@@ -611,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U37" sqref="U37"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,13 +652,13 @@
         <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>53</v>
+        <v>88</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>54</v>
+        <v>89</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>23</v>
@@ -694,7 +697,7 @@
         <v>44</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -705,7 +708,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -756,7 +759,7 @@
         <v>51</v>
       </c>
       <c r="T2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -767,7 +770,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>9</v>
@@ -818,7 +821,7 @@
         <v>51</v>
       </c>
       <c r="T3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -829,7 +832,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>10</v>
@@ -880,7 +883,7 @@
         <v>51</v>
       </c>
       <c r="T4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -891,7 +894,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -942,7 +945,7 @@
         <v>51</v>
       </c>
       <c r="T5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -953,7 +956,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>12</v>
@@ -1004,18 +1007,18 @@
         <v>51</v>
       </c>
       <c r="T6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
+      <c r="A7" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>12</v>
@@ -1066,7 +1069,7 @@
         <v>51</v>
       </c>
       <c r="T7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -1077,7 +1080,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>12</v>
@@ -1128,7 +1131,7 @@
         <v>51</v>
       </c>
       <c r="T8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -1139,7 +1142,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>12</v>
@@ -1190,7 +1193,7 @@
         <v>51</v>
       </c>
       <c r="T9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -1201,7 +1204,7 @@
         <v>0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>12</v>
@@ -1252,7 +1255,7 @@
         <v>51</v>
       </c>
       <c r="T10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -1263,7 +1266,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>12</v>
@@ -1314,7 +1317,7 @@
         <v>51</v>
       </c>
       <c r="T11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -1325,7 +1328,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>12</v>
@@ -1376,7 +1379,7 @@
         <v>51</v>
       </c>
       <c r="T12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -1387,7 +1390,7 @@
         <v>0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>12</v>
@@ -1438,7 +1441,7 @@
         <v>51</v>
       </c>
       <c r="T13" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -1449,7 +1452,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>12</v>
@@ -1500,7 +1503,7 @@
         <v>51</v>
       </c>
       <c r="T14" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
@@ -1511,7 +1514,7 @@
         <v>0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>12</v>
@@ -1562,7 +1565,7 @@
         <v>51</v>
       </c>
       <c r="T15" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -1594,7 +1597,7 @@
         <v>51</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>51</v>
@@ -1624,7 +1627,7 @@
         <v>51</v>
       </c>
       <c r="T16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
@@ -1656,7 +1659,7 @@
         <v>51</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>29</v>
@@ -1686,7 +1689,7 @@
         <v>51</v>
       </c>
       <c r="T17" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
@@ -1718,7 +1721,7 @@
         <v>51</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>30</v>
@@ -1748,7 +1751,7 @@
         <v>51</v>
       </c>
       <c r="T18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
@@ -1780,7 +1783,7 @@
         <v>51</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>30</v>
@@ -1810,7 +1813,7 @@
         <v>51</v>
       </c>
       <c r="T19" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
@@ -1842,7 +1845,7 @@
         <v>51</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>30</v>
@@ -1872,7 +1875,7 @@
         <v>51</v>
       </c>
       <c r="T20" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
@@ -1934,7 +1937,7 @@
         <v>51</v>
       </c>
       <c r="T21" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
@@ -1996,7 +1999,7 @@
         <v>51</v>
       </c>
       <c r="T22" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
@@ -2058,7 +2061,7 @@
         <v>51</v>
       </c>
       <c r="T23" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
@@ -2120,7 +2123,7 @@
         <v>51</v>
       </c>
       <c r="T24" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
@@ -2131,7 +2134,7 @@
         <v>0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>51</v>
@@ -2167,10 +2170,10 @@
         <v>51</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="Q25" s="1" t="s">
         <v>51</v>
@@ -2182,7 +2185,7 @@
         <v>51</v>
       </c>
       <c r="T25" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
@@ -2193,7 +2196,7 @@
         <v>0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>51</v>
@@ -2229,7 +2232,7 @@
         <v>51</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="P26" s="1" t="s">
         <v>51</v>
@@ -2244,7 +2247,7 @@
         <v>51</v>
       </c>
       <c r="T26" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
@@ -2255,7 +2258,7 @@
         <v>0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>51</v>
@@ -2291,10 +2294,10 @@
         <v>51</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="Q27" s="1" t="s">
         <v>51</v>
@@ -2306,7 +2309,7 @@
         <v>51</v>
       </c>
       <c r="T27" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
@@ -2359,7 +2362,7 @@
         <v>51</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="R28" s="1" t="s">
         <v>51</v>
@@ -2368,7 +2371,7 @@
         <v>47</v>
       </c>
       <c r="T28" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
@@ -2421,7 +2424,7 @@
         <v>51</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="R29" s="1" t="s">
         <v>51</v>
@@ -2430,7 +2433,7 @@
         <v>45</v>
       </c>
       <c r="T29" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
@@ -2483,7 +2486,7 @@
         <v>51</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="R30" s="1" t="s">
         <v>51</v>
@@ -2492,7 +2495,7 @@
         <v>46</v>
       </c>
       <c r="T30" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
@@ -2545,7 +2548,7 @@
         <v>51</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="R31" s="1" t="s">
         <v>48</v>
@@ -2554,7 +2557,7 @@
         <v>51</v>
       </c>
       <c r="T31" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
@@ -2607,7 +2610,7 @@
         <v>51</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="R32" s="1" t="s">
         <v>49</v>
@@ -2616,7 +2619,7 @@
         <v>51</v>
       </c>
       <c r="T32" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>